<commit_message>
-Update results 005 - 011
</commit_message>
<xml_diff>
--- a/20160411 - 006/running_logs/logs.xlsx
+++ b/20160411 - 006/running_logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
   <si>
     <t>Time</t>
   </si>
@@ -43,103 +43,58 @@
     <t>Template Filter</t>
   </si>
   <si>
-    <t>20160412_113609</t>
-  </si>
-  <si>
-    <t>remove break line, space after punctuation, convert to lower, remove multiple spaces, convert unicode to ascii, trim "space" and ","</t>
-  </si>
-  <si>
-    <t>10 features: #ascii/(#ascii+#digit+#punctuation), #digit/(#ascii+#digit+#punctuation), %kwName, %kwAddress, %kwPhone, %max_digit_skip_0, first_character_ascii, first_character_digit, last_character_ascii, last_character_digit</t>
+    <t>20160414_100653</t>
+  </si>
+  <si>
+    <t>convert to lower, convert unicode to ascii, trim "space" and ",", space after punctuation, remove multiple spaces, remove break line</t>
+  </si>
+  <si>
+    <t>12 features: length, #ascii/(#ascii+#digit+#punctuation), #digit/(#ascii+#digit+#punctuation), #digit/#ascii, %kwName, %kwAddress, %kwPhone, %max_digit_skip_0, first_character_ascii, first_character_digit, last_character_ascii, last_character_digit</t>
   </si>
   <si>
     <t>Neuron Network</t>
   </si>
   <si>
-    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 10</t>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 100</t>
+  </si>
+  <si>
+    <t>0 filters:</t>
+  </si>
+  <si>
+    <t>20160414_101023</t>
+  </si>
+  <si>
+    <t>20160414_101418</t>
+  </si>
+  <si>
+    <t>20160414_101751</t>
+  </si>
+  <si>
+    <t>20160414_102102</t>
+  </si>
+  <si>
+    <t>20160415_171134</t>
+  </si>
+  <si>
+    <t>trim "space" and ",", remove break line, remove multiple spaces, convert unicode to ascii, space after punctuation, convert to lower</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 300</t>
   </si>
   <si>
     <t xml:space="preserve">0 filters: </t>
   </si>
   <si>
-    <t>20160412_114808</t>
-  </si>
-  <si>
-    <t>trim "space" and ",", space after punctuation, convert unicode to ascii, remove multiple spaces, convert to lower, remove break line</t>
-  </si>
-  <si>
-    <t>11 features: #ascii/(#ascii+#digit+#punctuation), #digit/(#ascii+#digit+#punctuation), #digit/#ascii, %kwName, %kwAddress, %kwPhone, %max_digit_skip_0, first_character_ascii, first_character_digit, last_character_ascii, last_character_digit</t>
-  </si>
-  <si>
-    <t>20160412_115133</t>
-  </si>
-  <si>
-    <t>space after punctuation, trim "space" and ",", convert to lower, remove multiple spaces, remove break line, convert unicode to ascii</t>
-  </si>
-  <si>
-    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 100</t>
-  </si>
-  <si>
-    <t>20160412_115612</t>
-  </si>
-  <si>
-    <t>trim "space" and ",", convert unicode to ascii, remove break line, convert to lower, remove multiple spaces, space after punctuation</t>
-  </si>
-  <si>
-    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 300</t>
-  </si>
-  <si>
-    <t>20160412_121511</t>
-  </si>
-  <si>
-    <t>convert unicode to ascii, remove multiple spaces, trim "space" and ",", convert to lower, space after punctuation, remove break line</t>
-  </si>
-  <si>
-    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 1000</t>
-  </si>
-  <si>
-    <t>20160412_124931</t>
-  </si>
-  <si>
-    <t>space after punctuation, remove break line, trim "space" and ",", convert to lower, convert unicode to ascii, remove multiple spaces</t>
-  </si>
-  <si>
-    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 2000</t>
-  </si>
-  <si>
-    <t>20160412_134429</t>
-  </si>
-  <si>
-    <t>remove multiple spaces, convert to lower, remove break line, convert unicode to ascii, trim "space" and ",", space after punctuation</t>
-  </si>
-  <si>
-    <t>20160412_144934</t>
-  </si>
-  <si>
-    <t>space after punctuation, remove multiple spaces, trim "space" and ",", convert to lower, convert unicode to ascii, remove break line</t>
-  </si>
-  <si>
-    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 3000</t>
-  </si>
-  <si>
-    <t>20160414_100653</t>
-  </si>
-  <si>
-    <t>convert to lower, convert unicode to ascii, trim "space" and ",", space after punctuation, remove multiple spaces, remove break line</t>
-  </si>
-  <si>
-    <t>12 features: length, #ascii/(#ascii+#digit+#punctuation), #digit/(#ascii+#digit+#punctuation), #digit/#ascii, %kwName, %kwAddress, %kwPhone, %max_digit_skip_0, first_character_ascii, first_character_digit, last_character_ascii, last_character_digit</t>
-  </si>
-  <si>
-    <t>20160414_101023</t>
-  </si>
-  <si>
-    <t>20160414_101418</t>
-  </si>
-  <si>
-    <t>20160414_101751</t>
-  </si>
-  <si>
-    <t>20160414_102102</t>
+    <t>20160415_171453</t>
+  </si>
+  <si>
+    <t>20160415_171906</t>
+  </si>
+  <si>
+    <t>20160415_172354</t>
+  </si>
+  <si>
+    <t>20160415_172909</t>
   </si>
 </sst>
 </file>
@@ -471,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -511,7 +466,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>26.892</v>
+        <v>210.168</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -526,7 +481,7 @@
         <v>13</v>
       </c>
       <c r="G2">
-        <v>0.948666666666667</v>
+        <v>0.999333333333333</v>
       </c>
       <c r="H2">
         <v>0.937293729372937</v>
@@ -535,7 +490,7 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <v>0.518518518518518</v>
+        <v>0.0759493670886076</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -543,13 +498,13 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>25.455</v>
+        <v>234.987</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -558,260 +513,260 @@
         <v>13</v>
       </c>
       <c r="G3">
-        <v>0.942</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0.927392739273927</v>
+        <v>0.933993399339934</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
       </c>
       <c r="J3">
-        <v>0.487179487179487</v>
+        <v>0.0769230769230769</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>112.605</v>
+        <v>212.297</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>0.972</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>0.940594059405941</v>
+        <v>0.933993399339934</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
       </c>
       <c r="J4">
-        <v>0.439024390243902</v>
+        <v>0.0769230769230769</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>375.688</v>
+        <v>190.864</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G5">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0.940594059405941</v>
+        <v>0.937293729372937</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
       </c>
       <c r="J5">
-        <v>0.390243902439024</v>
+        <v>0.0886075949367089</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>814.171</v>
+        <v>208.347</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="G6">
-        <v>0.985333333333333</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0.940594059405941</v>
+        <v>0.933993399339934</v>
       </c>
       <c r="I6" t="s">
         <v>14</v>
       </c>
       <c r="J6">
-        <v>0.585365853658537</v>
+        <v>0.0897435897435897</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B7">
-        <v>1905.992</v>
+        <v>198.666</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G7">
-        <v>0.994</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0.940594059405941</v>
+        <v>0.933993399339934</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J7">
-        <v>0.682926829268293</v>
+        <v>0.115384615384615</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>1976.679</v>
+        <v>252.985</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G8">
-        <v>0.996</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>0.940594059405941</v>
+        <v>0.933993399339934</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J8">
-        <v>0.560975609756098</v>
+        <v>0.115384615384615</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B9">
-        <v>2639.888</v>
+        <v>288.741</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G9">
-        <v>0.996</v>
+        <v>0.998</v>
       </c>
       <c r="H9">
-        <v>0.940594059405941</v>
+        <v>0.943894389438944</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J9">
-        <v>0.585365853658537</v>
+        <v>0.0740740740740741</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B10">
-        <v>210.168</v>
+        <v>314.434</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10">
-        <v>0.999333333333333</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0.937293729372937</v>
+        <v>0.933993399339934</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J10">
-        <v>0.0759493670886076</v>
+        <v>0.102564102564103</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B11">
-        <v>234.987</v>
+        <v>346.333</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -820,106 +775,10 @@
         <v>0.933993399339934</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J11">
-        <v>0.0769230769230769</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12">
-        <v>212.297</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0.933993399339934</v>
-      </c>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12">
-        <v>0.0769230769230769</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13">
-        <v>190.864</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0.937293729372937</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13">
-        <v>0.0886075949367089</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14">
-        <v>208.347</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0.933993399339934</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14">
-        <v>0.0897435897435897</v>
+        <v>0.115384615384615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more results 006 and 011
</commit_message>
<xml_diff>
--- a/20160411 - 006/running_logs/logs.xlsx
+++ b/20160411 - 006/running_logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
   <si>
     <t>Time</t>
   </si>
@@ -95,6 +95,27 @@
   </si>
   <si>
     <t>20160415_172909</t>
+  </si>
+  <si>
+    <t>20160418_074607</t>
+  </si>
+  <si>
+    <t>convert to lower, space after punctuation, convert unicode to ascii, trim "space" and ",", remove break line, remove multiple spaces</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 1000</t>
+  </si>
+  <si>
+    <t>20160418_075604</t>
+  </si>
+  <si>
+    <t>20160418_080559</t>
+  </si>
+  <si>
+    <t>20160418_081601</t>
+  </si>
+  <si>
+    <t>20160418_082608</t>
   </si>
 </sst>
 </file>
@@ -426,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -781,6 +802,166 @@
         <v>0.115384615384615</v>
       </c>
     </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>597.354</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12">
+        <v>0.999333333333333</v>
+      </c>
+      <c r="H12">
+        <v>0.95049504950495</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12">
+        <v>0.180722891566265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>594.869</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0.943894389438944</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13">
+        <v>0.222222222222222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>601.867</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0.943894389438944</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14">
+        <v>0.185185185185185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>607.28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0.943894389438944</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15">
+        <v>0.172839506172839</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>623.781</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0.943894389438944</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16">
+        <v>0.160493827160494</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>